<commit_message>
Template: Partita iva gestita come testo
</commit_message>
<xml_diff>
--- a/dati_template.xlsx
+++ b/dati_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Spese" sheetId="1" r:id="rId1"/>
@@ -117,11 +117,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -404,7 +405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -487,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,7 +518,7 @@
       <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="4">
         <v>65498732105</v>
       </c>
     </row>
@@ -525,7 +526,7 @@
       <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="4">
         <v>3489543096</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Nuova versione: formato excel + nuovi campi
</commit_message>
<xml_diff>
--- a/dati_template.xlsx
+++ b/dati_template.xlsx
@@ -1,45 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\sistemats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A25DE00-3CE5-4792-907F-39BD2FBCB99A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5B25C5-C0D3-450E-8D58-5AA763C91F92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="15" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Spese" sheetId="1" r:id="rId1"/>
-    <sheet name="Dati personali" sheetId="2" r:id="rId2"/>
+    <sheet name="Fatture" sheetId="1" r:id="rId1"/>
+    <sheet name="Sistema TS" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>dataEmissione</t>
-  </si>
-  <si>
-    <t>numDocumento</t>
-  </si>
-  <si>
-    <t>dataPagamento</t>
-  </si>
-  <si>
-    <t>codiceFiscaleCliente</t>
-  </si>
-  <si>
-    <t>importo</t>
-  </si>
-  <si>
-    <t>protocollo</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>P1993</t>
   </si>
@@ -71,13 +53,58 @@
     <t>pincode</t>
   </si>
   <si>
-    <t>pagamentoTracciato</t>
-  </si>
-  <si>
     <t>SI</t>
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>naturaPrestazione</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>naturaBollo</t>
+  </si>
+  <si>
+    <t>N1</t>
+  </si>
+  <si>
+    <t>tipoSpesa</t>
+  </si>
+  <si>
+    <t>N2.2</t>
+  </si>
+  <si>
+    <t>DATA</t>
+  </si>
+  <si>
+    <t>N FATTURA</t>
+  </si>
+  <si>
+    <t>DATA PAGAMENTO</t>
+  </si>
+  <si>
+    <t>C.F.</t>
+  </si>
+  <si>
+    <t>NETTO PAGARE</t>
+  </si>
+  <si>
+    <t>TRACCIATO</t>
+  </si>
+  <si>
+    <t>PROTOCOLLO</t>
+  </si>
+  <si>
+    <t>OPPOSIZIONE</t>
+  </si>
+  <si>
+    <t>N. MARCA</t>
+  </si>
+  <si>
+    <t>9127341836189</t>
   </si>
 </sst>
 </file>
@@ -127,13 +154,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -427,76 +455,92 @@
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="22.44140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="75.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="22.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="75.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>42370</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C2" s="2">
         <v>42370</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>55.6</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>42370</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2">
         <v>42370</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E3">
         <v>5312.6</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
     </row>
   </sheetData>
@@ -507,37 +551,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="F19:G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B3" s="4">
         <v>65498732105</v>
@@ -545,13 +589,38 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B4" s="4">
         <v>3489543096</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>